<commit_message>
added notifications, added some TODO
</commit_message>
<xml_diff>
--- a/nycitybot.xlsx
+++ b/nycitybot.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matth\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matth\Documents\Code\JavaScript1.8 et NodeJs\nycitybot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B75ACE-A39E-4274-9512-2C4CAB0C91C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74AEE3C-2AED-4129-9ACC-05632D178D95}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{D6280C26-08CD-4AFB-8829-C3F2B1632DD5}"/>
   </bookViews>
@@ -241,35 +241,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8585"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -295,34 +267,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8585"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -643,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6841A06A-223D-4CCA-916A-0C3BF39DE21D}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>37</v>
@@ -725,10 +669,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,24 +1035,24 @@
         <v>41</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="pas encore fait">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="pas encore fait">
       <formula>NOT(ISERROR(SEARCH("pas encore fait",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="non">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="non">
       <formula>NOT(ISERROR(SEARCH("non",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>